<commit_message>
Prices for components updated
added unit price for due and tranceivers plus shipping
</commit_message>
<xml_diff>
--- a/Documentation/Bill of Materials.xlsx
+++ b/Documentation/Bill of Materials.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chad\Documents\GitHub\DigitalDash\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="70" windowWidth="10500" windowHeight="2340"/>
+    <workbookView xWindow="14640" yWindow="75" windowWidth="10500" windowHeight="2340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name of Component</t>
   </si>
@@ -37,12 +42,24 @@
   </si>
   <si>
     <t>MCP2551 transceivers</t>
+  </si>
+  <si>
+    <t>Shipping</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Arduino-A000062-Due/dp/B00A6C3JN2/ref=sr_1_1?ie=UTF8&amp;qid=1422406211&amp;sr=8-1&amp;keywords=arduino+due&amp;pebp=1422406212053&amp;peasin=B00A6C3JN2</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?KeyWords=MCP2551-I%2FP-ND%20&amp;WT.z_header=search_go</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -94,13 +111,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -110,6 +128,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -158,7 +179,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -193,7 +214,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -402,19 +423,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.36328125" customWidth="1"/>
-    <col min="5" max="5" width="18.26953125" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -425,31 +450,125 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="B2" s="4">
+        <v>47.5</v>
+      </c>
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D2" s="4">
+        <v>8.99</v>
+      </c>
+      <c r="E2" s="4">
+        <f>(B2*C2)+D2</f>
+        <v>56.49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="B3" s="4">
+        <v>1.22</v>
+      </c>
       <c r="C3">
         <v>2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>5.23</v>
+      </c>
+      <c r="E3" s="4">
+        <f>(B3*C3)+D3</f>
+        <v>7.67</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4">
+        <f>SUM(B4:D4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4">
+        <f t="shared" ref="E5:E11" si="0">SUM(B5:D5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="E10" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="E11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E3" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -459,7 +578,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -471,7 +590,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>